<commit_message>
Nightly Commit and Push
Drawing the Sun, Earth, and Moon. FPS camera is functional. Point light is functional.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED0F2DE-A7E6-4162-AC1D-D2AD9AC8658A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46972000-EA2F-48AB-8C59-83F60D3BFE28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -936,7 +939,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1073,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1078,7 +1081,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1094,11 +1097,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1219,7 +1226,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -2484,11 +2491,15 @@
       <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -2953,11 +2964,15 @@
       <c r="D84" s="5">
         <v>4</v>
       </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="3"/>
+      <c r="E84" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G84" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
@@ -3099,7 +3114,9 @@
       <c r="D91" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3121,7 +3138,9 @@
       <c r="D92" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E92" s="3"/>
+      <c r="E92" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
@@ -3254,7 +3273,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Commit for Milestone 3
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA89B0EC-DD71-4107-A8CE-00F123F20675}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AC7433-C179-4996-A274-3F412C78DAFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -939,7 +939,7 @@
   <dimension ref="A1:L118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,15 +1073,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1134,11 +1134,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
@@ -1150,7 +1154,7 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
@@ -1218,7 +1222,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
@@ -1226,7 +1230,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -3285,7 +3289,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Initial Commit for class retake
Commit before submitting new excel rubric for ppiv retake.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AC7433-C179-4996-A274-3F412C78DAFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CEA847-99EE-448D-A85C-E4215B61360E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Manually adjustable camera zoom level. Must be smooth and capped to a min and max value.</t>
   </si>
   <si>
-    <t>Student Git Address:  https://github.com/maximusrex17/PPIV_Repo</t>
-  </si>
-  <si>
     <t>Student Name: Joseph Gill</t>
   </si>
   <si>
@@ -341,10 +338,10 @@
     <t>I</t>
   </si>
   <si>
-    <t>II</t>
-  </si>
-  <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>Student Git Address:  https://github.com/maximusrex17/Project4</t>
   </si>
 </sst>
 </file>
@@ -938,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +955,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -974,7 +971,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1054,34 +1051,34 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1098,14 +1095,14 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1134,19 +1131,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>102</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
@@ -1154,7 +1147,7 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
@@ -1176,10 +1169,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
@@ -1211,10 +1204,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
@@ -1222,15 +1215,15 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1249,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
@@ -1291,7 +1284,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
@@ -1418,10 +1411,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
@@ -1536,10 +1529,10 @@
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
@@ -1615,10 +1608,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
@@ -1958,10 +1951,10 @@
         <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
@@ -2376,10 +2369,10 @@
         <v>2</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
@@ -2508,10 +2501,10 @@
         <v>2</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
@@ -2981,10 +2974,10 @@
         <v>4</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G84" s="16">
         <f t="shared" si="1"/>
@@ -3125,14 +3118,10 @@
         <v>2</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3149,14 +3138,10 @@
         <v>1</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
@@ -3289,7 +3274,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
End of lab Commit
Added functional Spot light and controls for said spot light. Started to work with multi view ports.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BDC1CE-4211-4A2D-96A4-64DB65893A07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB3F594-F1A1-4AA0-AC3A-A5FC8DD0A14D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,15 +1073,15 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1134,11 +1134,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
@@ -1150,12 +1154,12 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1226,7 +1230,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1279,23 +1283,27 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -3305,7 +3313,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Final commit for milestone 3
Added render to texture, press 2 to switch scenes and hold shift and move the mouse  to rotate the camera
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB3F594-F1A1-4AA0-AC3A-A5FC8DD0A14D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B852C94-EAD1-4D62-B372-66A0AC68CA31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,11 +1077,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1154,12 +1154,12 @@
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 60, SUM(-60,L4),0)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1295,15 +1295,15 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1601,11 +1601,15 @@
       <c r="D23" s="5">
         <v>4</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G23" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -3313,7 +3317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>